<commit_message>
CCSB Loads, Combined Outflow, 11452901, wy2016-18, SSC and fMeHg: updated model stats; new folders in rloadest; updated Sigma Plot file and PowerPoint files; added new PDF files to Sigma Plot folder; updated Loads Progress sheet.
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/4_wy2016-2018/4_SSC Model Results.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/4_wy2016-2018/4_SSC Model Results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Model Stats_rloadest\4_wy2016-2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598C7C1C-2A46-41C2-A59C-84757133988D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756ABE5A-210E-4BCC-B142-CA28AAD6CE77}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSC wy2016-18 Model Results" sheetId="2" r:id="rId1"/>
-    <sheet name="Outlet_30ct" sheetId="5" r:id="rId2"/>
-    <sheet name="Rumsey" sheetId="8" r:id="rId3"/>
+    <sheet name="Combined" sheetId="9" r:id="rId2"/>
+    <sheet name="Outlet_30ct" sheetId="5" r:id="rId3"/>
+    <sheet name="Rumsey" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="663">
   <si>
     <t>Model #</t>
   </si>
@@ -1462,6 +1463,603 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 36; Period of record: 2016-01-20 to 2018-04-08</t>
+  </si>
+  <si>
+    <t>Combined Outflow SSC</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(1), data = SSC_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(2), data = SSC_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(3), data = SSC_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(4), data = SSC_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(5), data = SSC_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(6), data = SSC_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(7), data = SSC_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(8), data = SSC_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(9), data = SSC_Combined, flow = "Flow", :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm1 &lt;- loadReg(SSC ~model(1), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(1), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Number of Observations: 36</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Center of Decimal Time: 2016.919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Center of ln(Q): 7.0238</t>
+  </si>
+  <si>
+    <t>(Intercept)   12.822     0.1696   75.62       0</t>
+  </si>
+  <si>
+    <t>lnQ            1.515     0.1003   15.10       0</t>
+  </si>
+  <si>
+    <t>Residual variance: 1.025</t>
+  </si>
+  <si>
+    <t>R-squared: 87.02 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 73.51 on 1 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9807</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.209</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.5647</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Min   25%     50%     75%      90%      95%      Max</t>
+  </si>
+  <si>
+    <t>Est 6140 83700 2330000 6860000 20100000 25400000 26200000</t>
+  </si>
+  <si>
+    <t>Obs 2710 64400  744000 5730000 14900000 22400000 35500000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 21.84 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7712</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm2 &lt;- loadReg(SSC ~model(2), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(2), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm2</t>
+  </si>
+  <si>
+    <t>(Intercept) 12.78806    0.27291 46.8580  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.51488    0.10180 14.8814  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.01204    0.07418  0.1623  0.8654</t>
+  </si>
+  <si>
+    <t>Residual variance: 1.055</t>
+  </si>
+  <si>
+    <t>R-squared: 87.03 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 73.54 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1832</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.5711</t>
+  </si>
+  <si>
+    <t>Est 6050 83300 2280000 6940000 20600000 26000000 26800000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 24.08 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7597</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm3 &lt;- loadReg(SSC ~model(3), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(3), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm3</t>
+  </si>
+  <si>
+    <t>(Intercept)   12.719    0.16698  76.166  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ            1.543    0.09573  16.118  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME       -0.620    0.27730  -2.236  0.0242</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.9172</t>
+  </si>
+  <si>
+    <t>R-squared: 88.73 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 78.59 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.9018</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4827</t>
+  </si>
+  <si>
+    <t>lnQ     1.017</t>
+  </si>
+  <si>
+    <t>DECTIME 1.017</t>
+  </si>
+  <si>
+    <t>Est 3880 65100 2040000 6970000 16300000 20300000 22500000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 6.516 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8136</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm4 &lt;- loadReg(SSC ~model(4), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(4), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm4</t>
+  </si>
+  <si>
+    <t>(Intercept)  11.4871     1.0118 11.3526  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.4337     0.1071 13.3854  0.0000</t>
+  </si>
+  <si>
+    <t>sin.DECTIME   0.7304     0.8868  0.8237  0.3848</t>
+  </si>
+  <si>
+    <t>cos.DECTIME   1.4936     0.8559  1.7451  0.0704</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.9442</t>
+  </si>
+  <si>
+    <t>R-squared: 88.75 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 78.65 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9664</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0346</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4444</t>
+  </si>
+  <si>
+    <t>lnQ         1.237</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 3.973</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 4.201</t>
+  </si>
+  <si>
+    <t>Est 9890 68600 1640000 7350000 21100000 23700000 26300000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 23.99 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7539</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm5 &lt;- loadReg(SSC ~model(5), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(5), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm5</t>
+  </si>
+  <si>
+    <t>(Intercept) 12.50480    0.28041 44.5949  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.54698    0.09597 16.1201  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.06952    0.07322  0.9495  0.3172</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.71046    0.29359 -2.4199  0.0139</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.92</t>
+  </si>
+  <si>
+    <t>R-squared: 89.04 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 79.59 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9902</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.6688</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4959</t>
+  </si>
+  <si>
+    <t>lnQ     1.019</t>
+  </si>
+  <si>
+    <t>lnQ2    1.118</t>
+  </si>
+  <si>
+    <t>DECTIME 1.137</t>
+  </si>
+  <si>
+    <t>Est 4330 64300 1710000 6950000 18800000 24400000 27400000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 17.24 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7996</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm6 &lt;- loadReg(SSC ~model(6), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(6), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm6</t>
+  </si>
+  <si>
+    <t>(Intercept) 11.63135    1.06931 10.8774  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.43311    0.10844 13.2152  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2        -0.03658    0.07779 -0.4703  0.6129</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  0.64758    0.91492  0.7078  0.4474</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  1.50643    0.86690  1.7377  0.0674</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.9677</t>
+  </si>
+  <si>
+    <t>R-squared: 88.83 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 78.91 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0214</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4202</t>
+  </si>
+  <si>
+    <t>lnQ         1.238</t>
+  </si>
+  <si>
+    <t>lnQ2        1.199</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 4.126</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 4.205</t>
+  </si>
+  <si>
+    <t>Est 7590 71800 1710000 7640000 18900000 20900000 23900000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 17.17 percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7974</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm7 &lt;- loadReg(SSC ~model(7), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(7), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Estimate Std. Error  z-score p-value</t>
+  </si>
+  <si>
+    <t>(Intercept) 12.31187     1.0836 11.36244  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.50099     0.1104 13.60181  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.54909     0.3088 -1.77837  0.0615</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -0.04015     0.9615 -0.04176  0.9641</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  0.72033     0.9355  0.76997  0.4089</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8844</t>
+  </si>
+  <si>
+    <t>R-squared: 89.79 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 82.15 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.142</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4278</t>
+  </si>
+  <si>
+    <t>lnQ         1.402</t>
+  </si>
+  <si>
+    <t>DECTIME     1.308</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 4.985</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.359</t>
+  </si>
+  <si>
+    <t>Est 3190 78000 1750000 6740000 16500000 23000000 26500000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 12.02 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8645</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm8 &lt;- loadReg(SSC ~model(8), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(8), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm8</t>
+  </si>
+  <si>
+    <t>(Intercept) 12.28770    1.10861 11.08389  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.50410    0.11337 13.26702  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.01504    0.08148  0.18457  0.8398</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.57246    0.33829 -1.69224  0.0700</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -0.03889    0.97681 -0.03981  0.9652</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  0.68213    0.97272  0.70126  0.4442</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.9129</t>
+  </si>
+  <si>
+    <t>R-squared: 89.8 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 82.19 on 5 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1427</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4356</t>
+  </si>
+  <si>
+    <t>lnQ         1.434</t>
+  </si>
+  <si>
+    <t>lnQ2        1.395</t>
+  </si>
+  <si>
+    <t>DECTIME     1.521</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 4.986</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.613</t>
+  </si>
+  <si>
+    <t>Est 3270 77200 1750000 6800000 17000000 23700000 27300000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 14.07 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8617</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm9 &lt;- loadReg(SSC ~model(9), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(9), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm9</t>
+  </si>
+  <si>
+    <t>(Intercept) 13.00038     1.1499 11.30574  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.67995     0.1496 11.22748  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.01531     0.0789  0.19410  0.8288</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.76027     0.3451 -2.20297  0.0183</t>
+  </si>
+  <si>
+    <t>DECTIME2     0.95074     0.5496  1.72972  0.0601</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -1.23398     1.1714 -1.05345  0.2449</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -0.01029     1.0235 -0.01005  0.9911</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.856</t>
+  </si>
+  <si>
+    <t>R-squared: 90.76 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 85.73 on 6 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9689</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0464</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4304</t>
+  </si>
+  <si>
+    <t>lnQ         2.664</t>
+  </si>
+  <si>
+    <t>DECTIME2    2.439</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 7.646</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 6.627</t>
+  </si>
+  <si>
+    <t>Est 4400 78300 1240000 7080000 15400000 29900000 33900000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 15.43 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8868</t>
+  </si>
+  <si>
+    <t>26.79, 27.20, 62.22</t>
+  </si>
+  <si>
+    <t>22.10, 27.55, 31.30</t>
   </si>
 </sst>
 </file>
@@ -1701,7 +2299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1821,6 +2419,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1849,7 +2456,127 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2382,11 +3109,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AE30"/>
+  <dimension ref="A1:AE43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O17" sqref="O17"/>
+      <selection pane="bottomLeft" activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2408,24 +3135,24 @@
       <c r="A1" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45" t="s">
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45" t="s">
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="45"/>
+      <c r="M1" s="48"/>
       <c r="O1" s="13"/>
       <c r="R1" s="13"/>
       <c r="S1" s="7" t="s">
@@ -2568,39 +3295,39 @@
       <c r="Q5" s="32"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="53" t="s">
         <v>267</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="52"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="55"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="50" t="s">
         <v>278</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="46" t="s">
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="46"/>
+      <c r="M7" s="49"/>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:31" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -3179,41 +3906,64 @@
       </c>
       <c r="AE17" s="8"/>
     </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" s="45"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+    </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B19" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="R19" s="1"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="53" t="s">
+        <v>465</v>
+      </c>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="O19" s="45"/>
+      <c r="P19" s="45"/>
+      <c r="R19" s="45"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B20" s="47" t="s">
-        <v>264</v>
-      </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="46" t="s">
+      <c r="A20" s="45"/>
+      <c r="B20" s="50" t="s">
+        <v>464</v>
+      </c>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="M20" s="46"/>
-      <c r="R20" s="1"/>
+      <c r="M20" s="49"/>
+      <c r="O20" s="45"/>
+      <c r="P20" s="45"/>
+      <c r="R20" s="45"/>
     </row>
     <row r="21" spans="1:31" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
@@ -3297,45 +4047,51 @@
         <v>7</v>
       </c>
       <c r="I22" s="6">
-        <v>91.51</v>
+        <v>87.02</v>
       </c>
       <c r="J22" s="6">
-        <v>0.80469999999999997</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="K22" s="6">
-        <v>0.57569999999999999</v>
+        <v>0.56469999999999998</v>
       </c>
       <c r="L22" s="6">
-        <v>78.040000000000006</v>
+        <v>21.84</v>
       </c>
       <c r="M22" s="6">
-        <v>-0.19059999999999999</v>
-      </c>
-      <c r="N22" s="27">
+        <v>0.7712</v>
+      </c>
+      <c r="N22" s="6">
         <v>1</v>
       </c>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
+      <c r="O22" s="27" t="s">
+        <v>459</v>
+      </c>
+      <c r="P22" s="27" t="s">
+        <v>662</v>
+      </c>
+      <c r="Q22" s="27" t="s">
+        <v>463</v>
+      </c>
       <c r="R22" s="7" t="s">
         <v>10</v>
       </c>
       <c r="T22" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD22" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="AB22" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="34">
+      <c r="A23" s="45">
         <v>2</v>
       </c>
       <c r="B23" s="6">
         <v>0</v>
       </c>
       <c r="C23" s="11">
-        <v>0.92269999999999996</v>
+        <v>0.86539999999999995</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>9</v>
@@ -3352,22 +4108,22 @@
       <c r="H23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I23" s="38">
-        <v>91.51</v>
-      </c>
-      <c r="J23" s="38">
-        <v>0.79710000000000003</v>
-      </c>
-      <c r="K23" s="38">
-        <v>0.57840000000000003</v>
-      </c>
-      <c r="L23" s="38">
-        <v>79.3</v>
-      </c>
-      <c r="M23" s="38">
-        <v>-0.2087</v>
-      </c>
-      <c r="N23" s="43">
+      <c r="I23" s="46">
+        <v>87.03</v>
+      </c>
+      <c r="J23" s="46">
+        <v>0.1832</v>
+      </c>
+      <c r="K23" s="46">
+        <v>0.57110000000000005</v>
+      </c>
+      <c r="L23" s="46">
+        <v>24.08</v>
+      </c>
+      <c r="M23" s="46">
+        <v>0.75970000000000004</v>
+      </c>
+      <c r="N23" s="45">
         <v>2</v>
       </c>
       <c r="O23" s="36"/>
@@ -3377,9 +4133,9 @@
         <v>10</v>
       </c>
       <c r="T23" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD23" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="AB23" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3394,7 +4150,7 @@
         <v>9</v>
       </c>
       <c r="D24" s="40">
-        <v>1E-4</v>
+        <v>2.4199999999999999E-2</v>
       </c>
       <c r="E24" s="39" t="s">
         <v>9</v>
@@ -3405,48 +4161,48 @@
       <c r="G24" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="35" t="s">
+      <c r="H24" s="47" t="s">
         <v>7</v>
       </c>
       <c r="I24" s="35">
-        <v>93.77</v>
+        <v>88.73</v>
       </c>
       <c r="J24" s="35">
-        <v>0.1643</v>
+        <v>0.90180000000000005</v>
       </c>
       <c r="K24" s="35">
-        <v>0.37240000000000001</v>
-      </c>
-      <c r="L24" s="27">
-        <v>30.74</v>
-      </c>
-      <c r="M24" s="27">
-        <v>0.66779999999999995</v>
+        <v>0.48270000000000002</v>
+      </c>
+      <c r="L24" s="35">
+        <v>6.516</v>
+      </c>
+      <c r="M24" s="35">
+        <v>0.81359999999999999</v>
       </c>
       <c r="N24" s="41">
         <v>3</v>
       </c>
       <c r="O24" s="41" t="s">
-        <v>265</v>
+        <v>459</v>
       </c>
       <c r="P24" s="41" t="s">
-        <v>266</v>
+        <v>661</v>
       </c>
       <c r="Q24" s="42" t="s">
-        <v>9</v>
+        <v>462</v>
       </c>
       <c r="R24" s="7" t="s">
         <v>10</v>
       </c>
       <c r="T24" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD24" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="AB24" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="34">
+      <c r="A25" s="45">
         <v>4</v>
       </c>
       <c r="B25" s="6">
@@ -3462,56 +4218,56 @@
         <v>9</v>
       </c>
       <c r="F25" s="6">
-        <v>0.1308</v>
-      </c>
-      <c r="G25" s="38">
-        <v>0.23449999999999999</v>
+        <v>0.38479999999999998</v>
+      </c>
+      <c r="G25" s="46">
+        <v>7.0400000000000004E-2</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I25" s="38">
-        <v>93.23</v>
-      </c>
-      <c r="J25" s="38">
-        <v>9.7000000000000003E-3</v>
-      </c>
-      <c r="K25" s="38">
-        <v>0.53649999999999998</v>
-      </c>
-      <c r="L25" s="38">
-        <v>87.43</v>
-      </c>
-      <c r="M25" s="38">
-        <v>-0.55110000000000003</v>
+      <c r="I25" s="46">
+        <v>88.75</v>
+      </c>
+      <c r="J25" s="46">
+        <v>3.4599999999999999E-2</v>
+      </c>
+      <c r="K25" s="46">
+        <v>0.44440000000000002</v>
+      </c>
+      <c r="L25" s="46">
+        <v>23.99</v>
+      </c>
+      <c r="M25" s="46">
+        <v>0.75390000000000001</v>
       </c>
       <c r="N25" s="27">
         <v>4</v>
       </c>
-      <c r="O25" s="34"/>
-      <c r="P25" s="34"/>
+      <c r="O25" s="45"/>
+      <c r="P25" s="45"/>
       <c r="R25" s="7" t="s">
         <v>10</v>
       </c>
       <c r="T25" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD25" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="AB25" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="34">
+      <c r="A26" s="45">
         <v>5</v>
       </c>
       <c r="B26" s="6">
         <v>0</v>
       </c>
-      <c r="C26" s="38">
-        <v>0.36209999999999998</v>
-      </c>
-      <c r="D26" s="38">
-        <v>0</v>
+      <c r="C26" s="46">
+        <v>0.31719999999999998</v>
+      </c>
+      <c r="D26" s="46">
+        <v>1.3899999999999999E-2</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>9</v>
@@ -3525,45 +4281,45 @@
       <c r="H26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I26" s="38">
-        <v>93.87</v>
-      </c>
-      <c r="J26" s="38">
-        <v>0.36049999999999999</v>
-      </c>
-      <c r="K26" s="38">
-        <v>0.37719999999999998</v>
-      </c>
-      <c r="L26" s="38">
-        <v>47.98</v>
-      </c>
-      <c r="M26" s="38">
-        <v>0.44280000000000003</v>
+      <c r="I26" s="46">
+        <v>89.04</v>
+      </c>
+      <c r="J26" s="46">
+        <v>0.66879999999999995</v>
+      </c>
+      <c r="K26" s="46">
+        <v>0.49590000000000001</v>
+      </c>
+      <c r="L26" s="46">
+        <v>17.239999999999998</v>
+      </c>
+      <c r="M26" s="46">
+        <v>0.79959999999999998</v>
       </c>
       <c r="N26" s="27">
         <v>5</v>
       </c>
-      <c r="O26" s="34"/>
-      <c r="P26" s="34"/>
+      <c r="O26" s="45"/>
+      <c r="P26" s="45"/>
       <c r="R26" s="7" t="s">
         <v>10</v>
       </c>
       <c r="T26" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD26" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="AB26" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="34">
+      <c r="A27" s="45">
         <v>6</v>
       </c>
       <c r="B27" s="6">
         <v>0</v>
       </c>
-      <c r="C27" s="38">
-        <v>0.56179999999999997</v>
+      <c r="C27" s="46">
+        <v>0.6129</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>9</v>
@@ -3572,46 +4328,46 @@
         <v>9</v>
       </c>
       <c r="F27" s="6">
-        <v>0.1792</v>
-      </c>
-      <c r="G27" s="38">
-        <v>0.187</v>
+        <v>0.44740000000000002</v>
+      </c>
+      <c r="G27" s="46">
+        <v>6.7400000000000002E-2</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I27" s="38">
-        <v>93.27</v>
-      </c>
-      <c r="J27" s="38">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="K27" s="38">
-        <v>0.51919999999999999</v>
-      </c>
-      <c r="L27" s="38">
-        <v>68.37</v>
-      </c>
-      <c r="M27" s="38">
-        <v>1.609E-2</v>
+      <c r="I27" s="46">
+        <v>88.83</v>
+      </c>
+      <c r="J27" s="46">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="K27" s="46">
+        <v>0.42020000000000002</v>
+      </c>
+      <c r="L27" s="46">
+        <v>17.170000000000002</v>
+      </c>
+      <c r="M27" s="46">
+        <v>0.7974</v>
       </c>
       <c r="N27" s="27">
         <v>6</v>
       </c>
-      <c r="O27" s="34"/>
-      <c r="P27" s="34"/>
+      <c r="O27" s="45"/>
+      <c r="P27" s="45"/>
       <c r="R27" s="7" t="s">
         <v>10</v>
       </c>
       <c r="T27" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD27" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="AB27" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="34">
+      <c r="A28" s="45">
         <v>7</v>
       </c>
       <c r="B28" s="6">
@@ -3621,229 +4377,879 @@
         <v>9</v>
       </c>
       <c r="D28" s="6">
-        <v>6.9999999999999999E-4</v>
+        <v>6.1499999999999999E-2</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F28" s="6">
-        <v>0.23760000000000001</v>
-      </c>
-      <c r="G28" s="38">
-        <v>0.33739999999999998</v>
+        <v>0.96409999999999996</v>
+      </c>
+      <c r="G28" s="46">
+        <v>0.40889999999999999</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="38">
-        <v>94.56</v>
-      </c>
-      <c r="J28" s="38">
-        <v>6.1600000000000002E-2</v>
-      </c>
-      <c r="K28" s="38">
-        <v>0.37819999999999998</v>
-      </c>
-      <c r="L28" s="38">
-        <v>41.42</v>
-      </c>
-      <c r="M28" s="38">
-        <v>0.50080000000000002</v>
+      <c r="I28" s="46">
+        <v>89.79</v>
+      </c>
+      <c r="J28" s="46">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="K28" s="46">
+        <v>0.42780000000000001</v>
+      </c>
+      <c r="L28" s="46">
+        <v>12.02</v>
+      </c>
+      <c r="M28" s="46">
+        <v>0.86450000000000005</v>
       </c>
       <c r="N28" s="27">
         <v>7</v>
       </c>
-      <c r="O28" s="34"/>
-      <c r="P28" s="34"/>
+      <c r="O28" s="45"/>
+      <c r="P28" s="45"/>
       <c r="R28" s="7" t="s">
         <v>10</v>
       </c>
       <c r="T28" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD28" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="AB28" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="34">
+      <c r="A29" s="45">
         <v>8</v>
       </c>
       <c r="B29" s="6">
         <v>0</v>
       </c>
-      <c r="C29" s="38">
-        <v>0.75829999999999997</v>
+      <c r="C29" s="46">
+        <v>0.83979999999999999</v>
       </c>
       <c r="D29" s="6">
-        <v>8.0000000000000004E-4</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F29" s="6">
-        <v>0.2228</v>
+        <v>0.96519999999999995</v>
       </c>
       <c r="G29" s="6">
-        <v>0.44800000000000001</v>
+        <v>0.44419999999999998</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I29" s="38">
-        <v>94.57</v>
-      </c>
-      <c r="J29" s="38">
-        <v>6.2300000000000001E-2</v>
-      </c>
-      <c r="K29" s="38">
-        <v>0.37940000000000002</v>
-      </c>
-      <c r="L29" s="38">
-        <v>46.59</v>
-      </c>
-      <c r="M29" s="38">
-        <v>0.4194</v>
+      <c r="I29" s="46">
+        <v>89.8</v>
+      </c>
+      <c r="J29" s="46">
+        <v>0.14269999999999999</v>
+      </c>
+      <c r="K29" s="46">
+        <v>0.43559999999999999</v>
+      </c>
+      <c r="L29" s="46">
+        <v>14.07</v>
+      </c>
+      <c r="M29" s="46">
+        <v>0.86170000000000002</v>
       </c>
       <c r="N29" s="27">
         <v>8</v>
       </c>
-      <c r="O29" s="34"/>
-      <c r="P29" s="34"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="45"/>
       <c r="R29" s="7" t="s">
         <v>10</v>
       </c>
       <c r="T29" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD29" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="AB29" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="34">
+      <c r="A30" s="45">
         <v>9</v>
       </c>
       <c r="B30" s="6">
         <v>0</v>
       </c>
-      <c r="C30" s="38">
-        <v>3.8800000000000001E-2</v>
+      <c r="C30" s="46">
+        <v>0.82879999999999998</v>
       </c>
       <c r="D30" s="6">
-        <v>6.9999999999999999E-4</v>
+        <v>1.83E-2</v>
       </c>
       <c r="E30" s="6">
-        <v>0</v>
+        <v>6.0100000000000001E-2</v>
       </c>
       <c r="F30" s="6">
-        <v>1E-4</v>
+        <v>0.24490000000000001</v>
       </c>
       <c r="G30" s="6">
-        <v>0.48080000000000001</v>
+        <v>0.99109999999999998</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I30" s="38">
-        <v>96.99</v>
-      </c>
-      <c r="J30" s="38">
-        <v>3.8E-3</v>
-      </c>
-      <c r="K30" s="38">
-        <v>5.9299999999999999E-2</v>
-      </c>
-      <c r="L30" s="38">
-        <v>45.01</v>
-      </c>
-      <c r="M30" s="38">
-        <v>0.17269999999999999</v>
+      <c r="I30" s="46">
+        <v>90.76</v>
+      </c>
+      <c r="J30" s="46">
+        <v>4.6399999999999997E-2</v>
+      </c>
+      <c r="K30" s="46">
+        <v>0.4304</v>
+      </c>
+      <c r="L30" s="46">
+        <v>15.43</v>
+      </c>
+      <c r="M30" s="46">
+        <v>0.88680000000000003</v>
       </c>
       <c r="N30" s="27">
         <v>9</v>
       </c>
-      <c r="O30" s="34"/>
-      <c r="P30" s="34"/>
+      <c r="O30" s="45"/>
+      <c r="P30" s="45"/>
       <c r="R30" s="7" t="s">
         <v>10</v>
       </c>
       <c r="T30" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="AB30" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B32" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="55"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="R32" s="1"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B33" s="50" t="s">
+        <v>264</v>
+      </c>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="M33" s="49"/>
+      <c r="R33" s="1"/>
+    </row>
+    <row r="34" spans="1:30" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="O34" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P34" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q34" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>1</v>
+      </c>
+      <c r="B35" s="6">
+        <v>0</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="6">
+        <v>91.51</v>
+      </c>
+      <c r="J35" s="6">
+        <v>0.80469999999999997</v>
+      </c>
+      <c r="K35" s="6">
+        <v>0.57569999999999999</v>
+      </c>
+      <c r="L35" s="6">
+        <v>78.040000000000006</v>
+      </c>
+      <c r="M35" s="6">
+        <v>-0.19059999999999999</v>
+      </c>
+      <c r="N35" s="27">
+        <v>1</v>
+      </c>
+      <c r="O35" s="27"/>
+      <c r="P35" s="27"/>
+      <c r="Q35" s="27"/>
+      <c r="R35" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T35" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD35" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="34">
+        <v>2</v>
+      </c>
+      <c r="B36" s="6">
+        <v>0</v>
+      </c>
+      <c r="C36" s="11">
+        <v>0.92269999999999996</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="38">
+        <v>91.51</v>
+      </c>
+      <c r="J36" s="38">
+        <v>0.79710000000000003</v>
+      </c>
+      <c r="K36" s="38">
+        <v>0.57840000000000003</v>
+      </c>
+      <c r="L36" s="38">
+        <v>79.3</v>
+      </c>
+      <c r="M36" s="38">
+        <v>-0.2087</v>
+      </c>
+      <c r="N36" s="43">
+        <v>2</v>
+      </c>
+      <c r="O36" s="36"/>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T36" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD36" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="35">
+        <v>3</v>
+      </c>
+      <c r="B37" s="35">
+        <v>0</v>
+      </c>
+      <c r="C37" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="40">
+        <v>1E-4</v>
+      </c>
+      <c r="E37" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="35">
+        <v>93.77</v>
+      </c>
+      <c r="J37" s="35">
+        <v>0.1643</v>
+      </c>
+      <c r="K37" s="35">
+        <v>0.37240000000000001</v>
+      </c>
+      <c r="L37" s="27">
+        <v>30.74</v>
+      </c>
+      <c r="M37" s="27">
+        <v>0.66779999999999995</v>
+      </c>
+      <c r="N37" s="41">
+        <v>3</v>
+      </c>
+      <c r="O37" s="41" t="s">
+        <v>265</v>
+      </c>
+      <c r="P37" s="41" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q37" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="R37" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T37" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD37" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="34">
+        <v>4</v>
+      </c>
+      <c r="B38" s="6">
+        <v>0</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="6">
+        <v>0.1308</v>
+      </c>
+      <c r="G38" s="38">
+        <v>0.23449999999999999</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="38">
+        <v>93.23</v>
+      </c>
+      <c r="J38" s="38">
+        <v>9.7000000000000003E-3</v>
+      </c>
+      <c r="K38" s="38">
+        <v>0.53649999999999998</v>
+      </c>
+      <c r="L38" s="38">
+        <v>87.43</v>
+      </c>
+      <c r="M38" s="38">
+        <v>-0.55110000000000003</v>
+      </c>
+      <c r="N38" s="27">
+        <v>4</v>
+      </c>
+      <c r="O38" s="34"/>
+      <c r="P38" s="34"/>
+      <c r="R38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T38" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD38" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="34">
+        <v>5</v>
+      </c>
+      <c r="B39" s="6">
+        <v>0</v>
+      </c>
+      <c r="C39" s="38">
+        <v>0.36209999999999998</v>
+      </c>
+      <c r="D39" s="38">
+        <v>0</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="38">
+        <v>93.87</v>
+      </c>
+      <c r="J39" s="38">
+        <v>0.36049999999999999</v>
+      </c>
+      <c r="K39" s="38">
+        <v>0.37719999999999998</v>
+      </c>
+      <c r="L39" s="38">
+        <v>47.98</v>
+      </c>
+      <c r="M39" s="38">
+        <v>0.44280000000000003</v>
+      </c>
+      <c r="N39" s="27">
+        <v>5</v>
+      </c>
+      <c r="O39" s="34"/>
+      <c r="P39" s="34"/>
+      <c r="R39" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T39" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD39" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="34">
+        <v>6</v>
+      </c>
+      <c r="B40" s="6">
+        <v>0</v>
+      </c>
+      <c r="C40" s="38">
+        <v>0.56179999999999997</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="6">
+        <v>0.1792</v>
+      </c>
+      <c r="G40" s="38">
+        <v>0.187</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="38">
+        <v>93.27</v>
+      </c>
+      <c r="J40" s="38">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="K40" s="38">
+        <v>0.51919999999999999</v>
+      </c>
+      <c r="L40" s="38">
+        <v>68.37</v>
+      </c>
+      <c r="M40" s="38">
+        <v>1.609E-2</v>
+      </c>
+      <c r="N40" s="27">
+        <v>6</v>
+      </c>
+      <c r="O40" s="34"/>
+      <c r="P40" s="34"/>
+      <c r="R40" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T40" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD40" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="34">
+        <v>7</v>
+      </c>
+      <c r="B41" s="6">
+        <v>0</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="6">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="6">
+        <v>0.23760000000000001</v>
+      </c>
+      <c r="G41" s="38">
+        <v>0.33739999999999998</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="38">
+        <v>94.56</v>
+      </c>
+      <c r="J41" s="38">
+        <v>6.1600000000000002E-2</v>
+      </c>
+      <c r="K41" s="38">
+        <v>0.37819999999999998</v>
+      </c>
+      <c r="L41" s="38">
+        <v>41.42</v>
+      </c>
+      <c r="M41" s="38">
+        <v>0.50080000000000002</v>
+      </c>
+      <c r="N41" s="27">
+        <v>7</v>
+      </c>
+      <c r="O41" s="34"/>
+      <c r="P41" s="34"/>
+      <c r="R41" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T41" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD41" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="34">
+        <v>8</v>
+      </c>
+      <c r="B42" s="6">
+        <v>0</v>
+      </c>
+      <c r="C42" s="38">
+        <v>0.75829999999999997</v>
+      </c>
+      <c r="D42" s="6">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="6">
+        <v>0.2228</v>
+      </c>
+      <c r="G42" s="6">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="38">
+        <v>94.57</v>
+      </c>
+      <c r="J42" s="38">
+        <v>6.2300000000000001E-2</v>
+      </c>
+      <c r="K42" s="38">
+        <v>0.37940000000000002</v>
+      </c>
+      <c r="L42" s="38">
+        <v>46.59</v>
+      </c>
+      <c r="M42" s="38">
+        <v>0.4194</v>
+      </c>
+      <c r="N42" s="27">
+        <v>8</v>
+      </c>
+      <c r="O42" s="34"/>
+      <c r="P42" s="34"/>
+      <c r="R42" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T42" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD42" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="34">
+        <v>9</v>
+      </c>
+      <c r="B43" s="6">
+        <v>0</v>
+      </c>
+      <c r="C43" s="38">
+        <v>3.8800000000000001E-2</v>
+      </c>
+      <c r="D43" s="6">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E43" s="6">
+        <v>0</v>
+      </c>
+      <c r="F43" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0.48080000000000001</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="38">
+        <v>96.99</v>
+      </c>
+      <c r="J43" s="38">
+        <v>3.8E-3</v>
+      </c>
+      <c r="K43" s="38">
+        <v>5.9299999999999999E-2</v>
+      </c>
+      <c r="L43" s="38">
+        <v>45.01</v>
+      </c>
+      <c r="M43" s="38">
+        <v>0.17269999999999999</v>
+      </c>
+      <c r="N43" s="27">
+        <v>9</v>
+      </c>
+      <c r="O43" s="34"/>
+      <c r="P43" s="34"/>
+      <c r="R43" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T43" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AD30" s="8" t="s">
+      <c r="AD43" s="8" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L32:M32"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B33:K33"/>
+    <mergeCell ref="B32:K32"/>
+    <mergeCell ref="B19:K19"/>
+    <mergeCell ref="L19:M19"/>
     <mergeCell ref="B20:K20"/>
-    <mergeCell ref="B19:K19"/>
+    <mergeCell ref="L20:M20"/>
   </mergeCells>
-  <conditionalFormatting sqref="M19 L55:L1048576">
-    <cfRule type="cellIs" dxfId="18" priority="64" operator="between">
+  <conditionalFormatting sqref="M32 L68:L1048576">
+    <cfRule type="cellIs" dxfId="30" priority="76" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="65" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="77" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="66" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="78" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19 K31:K1048576">
-    <cfRule type="cellIs" dxfId="15" priority="50" operator="lessThan">
+  <conditionalFormatting sqref="L32 K44:K1048576">
+    <cfRule type="cellIs" dxfId="27" priority="62" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="51" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="63" operator="greaterThan">
+      <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J35:J43">
+    <cfRule type="cellIs" dxfId="25" priority="41" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M35:M43">
+    <cfRule type="cellIs" dxfId="24" priority="45" operator="between">
+      <formula>0.5</formula>
+      <formula>0.8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="46" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="47" operator="greaterThan">
+      <formula>0.8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L35:L43">
+    <cfRule type="cellIs" dxfId="21" priority="43" operator="lessThan">
+      <formula>-25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="44" operator="greaterThan">
+      <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36 D37 C39:C40 D39 C42:C43 D41:D43 E43 F38:G38 F40:G43">
+    <cfRule type="cellIs" dxfId="19" priority="42" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:J17">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M9:M17">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="between">
+      <formula>0.5</formula>
+      <formula>0.8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="greaterThan">
+      <formula>0.8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:L17">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
+      <formula>-25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="greaterThan">
+      <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10 D11 C13:C14 D13 C16:C17 D15:D17 E17 F12:G12 F14:G17">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M19">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="between">
+      <formula>0.5</formula>
+      <formula>0.8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
+      <formula>0.8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
+      <formula>-25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:J30">
-    <cfRule type="cellIs" dxfId="13" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M22:M30">
-    <cfRule type="cellIs" dxfId="12" priority="33" operator="between">
-      <formula>0.5</formula>
-      <formula>0.8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="34" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="35" operator="greaterThan">
-      <formula>0.8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L22:L30">
-    <cfRule type="cellIs" dxfId="9" priority="31" operator="lessThan">
-      <formula>-25</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="32" operator="greaterThan">
-      <formula>25</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23 D24 C26:C27 D26 C29:C30 D28:D30 E30 F25:G25 F27:G30">
-    <cfRule type="cellIs" dxfId="7" priority="30" operator="greaterThan">
-      <formula>0.1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:J17">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
-      <formula>0.05</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M9:M17">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
@@ -3855,7 +5261,7 @@
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L9:L17">
+  <conditionalFormatting sqref="L22:L30">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
@@ -3863,7 +5269,7 @@
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10 D11 C13:C14 D13 C16:C17 D15:D17 E17 F12:G12 F14:G17">
+  <conditionalFormatting sqref="C23 D24 C26:C27 D26 C29:C30 D28:D30 E30 F25:G25 F27:G30">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
@@ -3875,6 +5281,2464 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6184FAB0-A70A-4282-BC63-337EADA57D1F}">
+  <dimension ref="A1:A524"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="22"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="24" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="24" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="22"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="24" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="24" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="24" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="22"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="23" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="23" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="22"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="22"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="24" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="24" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="24" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="24" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="22"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="22"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="22"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="24" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="24" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="24" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="22"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="24" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="24" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="24" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="24" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="24" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="24" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="22"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="22"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="24" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="24" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="22"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="24" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="24" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="24" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="22"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="23" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="7" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="23" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="22"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="24" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="22"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="24" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="24" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="24" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="24" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="22"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="22"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="22"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="24" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="24" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="24" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="22"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="24" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="24" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="24" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="24" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="24" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="24" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="22"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="24" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="24" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="22"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="24" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="24" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="22"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="24" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="24" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="24" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="22"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="23" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="7" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="23" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="22"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="24" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="22"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="24" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="24" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="24" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="24" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="22"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="22"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="22"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="24" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="24" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="24" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="24" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="22"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="24" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="24" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="24" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="24" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="24" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="24" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="22"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="24" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="24" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="24" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="22"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="24" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="24" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="22"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="24" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="24" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="24" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="22"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="23" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="7" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="23" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="22"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="24" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="22"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="24" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="24" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="24" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="24" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="22"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="22"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="22"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="24" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="24" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="24" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="24" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="22"/>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="24" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="24" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="24" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="24" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="24" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="24" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="22"/>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="24" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="24" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="24" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="22"/>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="24" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="24" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="22"/>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="24" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="24" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="24" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="22"/>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="23" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="7" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="23" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="22"/>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="24" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="22"/>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="24" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="24" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="24" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="24" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="22"/>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="22"/>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="24" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="22"/>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="24" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" s="24" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="24" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="24" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="24" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="22"/>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="24" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="24" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="24" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="24" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" s="24" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" s="24" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" s="22"/>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" s="24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" s="24" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" s="24" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" s="24" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" s="24" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" s="22"/>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" s="24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" s="24" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" s="24" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" s="22"/>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" s="24" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="24" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" s="24" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" s="22"/>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" s="23" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" s="7" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" s="23" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" s="22"/>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" s="24" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" s="22"/>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" s="24" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" s="24" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" s="24" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" s="24" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" s="22"/>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" s="22"/>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" s="24" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" s="22"/>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" s="24" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" s="24" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" s="24" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" s="24" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" s="24" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" s="24" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" s="22"/>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" s="24" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" s="24" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" s="24" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" s="24" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" s="24" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" s="24" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" s="22"/>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" s="24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" s="24" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" s="24" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" s="24" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" s="24" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" s="22"/>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" s="24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" s="24" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" s="24" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" s="22"/>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" s="24" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" s="24" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" s="24" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" s="22"/>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" s="23" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" s="7" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" s="23" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" s="22"/>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" s="24" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" s="22"/>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" s="24" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" s="24" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" s="24" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" s="24" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" s="22"/>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" s="22"/>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" s="24" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" s="22"/>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" s="24" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" s="24" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" s="24" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" s="24" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" s="24" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" s="24" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" s="24" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" s="22"/>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" s="24" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" s="24" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" s="24" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" s="24" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" s="24" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" s="24" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" s="22"/>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" s="24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" s="24" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" s="24" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" s="24" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" s="24" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" s="24" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" s="22"/>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" s="24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" s="24" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" s="24" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" s="22"/>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" s="24" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" s="24" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" s="24" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" s="22"/>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" s="23" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" s="7" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" s="23" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" s="22"/>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" s="24" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" s="22"/>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" s="24" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" s="24" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" s="24" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" s="24" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" s="22"/>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" s="22"/>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" s="24" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" s="22"/>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" s="24" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" s="24" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" s="24" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" s="24" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" s="24" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489" s="24" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" s="24" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" s="24" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" s="22"/>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" s="24" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" s="24" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" s="24" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" s="24" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" s="24" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" s="24" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" s="22"/>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" s="24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" s="24" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" s="24" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" s="24" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" s="24" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" s="24" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" s="24" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" s="22"/>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" s="24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" s="24" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" s="24" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" s="22"/>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" s="24" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" s="24" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" s="25" t="s">
+        <v>660</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E8CF0D-1596-4A2F-A50C-9BD320018867}">
   <dimension ref="A1:A524"/>
   <sheetViews>
@@ -6332,7 +10196,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7110874D-1AB5-4D4C-BDF4-3EDF5D1201E0}">
   <dimension ref="A1:A524"/>
   <sheetViews>

</xml_diff>